<commit_message>
Add rocker switch to BOM
</commit_message>
<xml_diff>
--- a/BOM 180823.xlsx
+++ b/BOM 180823.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Rob\Dropbox\Dropbox\rob\Repository\Mobile-APRS-Digipeater\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E9002C6B-1601-49B5-91B4-608232271F06}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{99E21736-4736-47B2-9497-7699EF85A8FA}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20040" windowHeight="17970" xr2:uid="{E06C1C2C-F7E2-4B46-BCA7-0CD26E66DCA6}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>Item</t>
   </si>
@@ -127,6 +127,12 @@
   </si>
   <si>
     <t>F2 crimp connectors for 12V battery</t>
+  </si>
+  <si>
+    <t>Rocker switch</t>
+  </si>
+  <si>
+    <t>https://smile.amazon.com/gp/product/B07D1J246N/ref=oh_aui_search_detailpage?ie=UTF8&amp;psc=1</t>
   </si>
 </sst>
 </file>
@@ -182,8 +188,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC5F62C9-FE37-4471-9A6E-5AB494510B88}" name="Table1" displayName="Table1" ref="A1:B20" totalsRowShown="0">
-  <autoFilter ref="A1:B20" xr:uid="{38778BE9-A7D5-4680-8140-57BEA5A02186}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC5F62C9-FE37-4471-9A6E-5AB494510B88}" name="Table1" displayName="Table1" ref="A1:B21" totalsRowShown="0">
+  <autoFilter ref="A1:B21" xr:uid="{38778BE9-A7D5-4680-8140-57BEA5A02186}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{66EDDD95-8FC7-4515-B1B4-C2214C4CC761}" name="Item"/>
     <tableColumn id="2" xr3:uid="{6B8DF500-83EB-4888-B9CE-40DA1276CB71}" name="URL"/>
@@ -489,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429C8022-5EB7-4F8D-91EA-27C96B2C05A6}">
-  <dimension ref="A1:B20"/>
+  <dimension ref="A1:B21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -616,39 +622,47 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>13</v>
+        <v>34</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B18" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="B19" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>4</v>
       </c>
-      <c r="B20" t="s">
+      <c r="B21" t="s">
         <v>5</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A2:B20">
-    <sortCondition ref="A2:A20"/>
+  <sortState ref="A2:B21">
+    <sortCondition ref="A2:A21"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">

</xml_diff>